<commit_message>
mise à jour 14/02
mise à jour du site
</commit_message>
<xml_diff>
--- a/Dossier/dictionnaire de donnée.xlsx
+++ b/Dossier/dictionnaire de donnée.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulb\OneDrive\Bureau\Portfolio Paul Berthelot\Dossier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulb\OneDrive\Bureau\paulberthelot-portfolio\Dossier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B65EAE-FB91-4B81-9430-6E09FD69EFA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E88256C-D5E9-439D-89C7-B2263B567F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6FCCB02-1440-4D2E-8C39-0CE3C91F6732}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{C6FCCB02-1440-4D2E-8C39-0CE3C91F6732}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Variable</t>
   </si>
@@ -78,7 +78,22 @@
     <t>elle contient les images</t>
   </si>
   <si>
-    <t>XXXXXXXXXXXXXXXXXXXXXXXXX</t>
+    <t>dl</t>
+  </si>
+  <si>
+    <t>slash</t>
+  </si>
+  <si>
+    <t>icône téléchargement</t>
+  </si>
+  <si>
+    <t>icône code slash</t>
+  </si>
+  <si>
+    <t>elle contient mon cv</t>
+  </si>
+  <si>
+    <t>XXXXXXXXXXXXXXXXXXXXXXXX</t>
   </si>
 </sst>
 </file>
@@ -464,7 +479,7 @@
   <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,7 +518,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -514,7 +529,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
@@ -525,7 +540,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
@@ -540,14 +555,26 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>

</xml_diff>